<commit_message>
rsab_fwd upload tested, incl sa_business dates
</commit_message>
<xml_diff>
--- a/Template_BondFwd.xlsx
+++ b/Template_BondFwd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Libfin\Staff\Jacob\Python Scripts\A2 Tickets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtm3004\Documents\Python Scripts\A2_Tickets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B6644B-8C85-4CEC-941D-938558C60895}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E61D0B-AD12-43CD-B631-D7CEE8FB0B73}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92BC32D5-4388-49D8-92A9-879D72B7F144}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92BC32D5-4388-49D8-92A9-879D72B7F144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>specificType</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>FOLLOWING</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5284C16A-6B93-4CDD-944A-AEEE0C8A8541}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,212 +543,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3">
-        <v>43929.5</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43929.5</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>-130</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>5.3999999999999902E-2</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.3999999999999902E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5">
-        <v>209</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B20" s="5">
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="3">
-        <v>43936.75</v>
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1000000</v>
+        <v>28</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43936.75</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1000000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.1168</v>
+        <v>32</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2">
-        <v>3</v>
+        <v>0.1168</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>